<commit_message>
need to test tx
</commit_message>
<xml_diff>
--- a/USB_STM32F4Cube_Base_project/calcs.xlsx
+++ b/USB_STM32F4Cube_Base_project/calcs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="55">
   <si>
     <t xml:space="preserve">#define CHANNR </t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>cc2400_en</t>
+  </si>
+  <si>
+    <t>group id</t>
+  </si>
+  <si>
+    <t>freq</t>
   </si>
 </sst>
 </file>
@@ -240,7 +246,17 @@
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -561,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,9 +589,10 @@
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D1" t="s">
         <v>29</v>
       </c>
@@ -585,8 +602,20 @@
       <c r="F1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1">
+        <v>2</v>
+      </c>
+      <c r="O1" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -603,8 +632,38 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2">
+        <f>(2400 + (I1)*8)/1000</f>
+        <v>2.4159999999999999</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O2" t="str">
+        <f>DEC2BIN(P2)</f>
+        <v>1011100</v>
+      </c>
+      <c r="P2">
+        <v>92</v>
+      </c>
+      <c r="Q2" t="str">
+        <f>DEC2HEX(P2)</f>
+        <v>5C</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -621,8 +680,28 @@
       <c r="E3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" t="str">
+        <f>DEC2BIN(P3)</f>
+        <v>11101100</v>
+      </c>
+      <c r="P3">
+        <v>236</v>
+      </c>
+      <c r="Q3" t="str">
+        <f t="shared" ref="Q3:Q4" si="1">DEC2HEX(P3)</f>
+        <v>EC</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -639,8 +718,28 @@
       <c r="E4" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" t="s">
+        <v>16</v>
+      </c>
+      <c r="O4" t="str">
+        <f>DEC2BIN(P4)</f>
+        <v>1001111</v>
+      </c>
+      <c r="P4">
+        <v>79</v>
+      </c>
+      <c r="Q4" t="str">
+        <f t="shared" si="1"/>
+        <v>4F</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -662,7 +761,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -677,14 +776,18 @@
         <v>10010100</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E7" si="1">HEX2DEC(F6)</f>
+        <f t="shared" ref="E6:E7" si="2">HEX2DEC(F6)</f>
         <v>148</v>
       </c>
       <c r="F6">
         <v>94</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <f>LEN(DEC2BIN(LARGE(P2:P4,1)))</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -699,14 +802,20 @@
         <v>10</v>
       </c>
       <c r="E7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -723,8 +832,17 @@
       <c r="E8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
+      <c r="N8">
+        <v>26</v>
+      </c>
+      <c r="O8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -741,8 +859,19 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" t="str">
+        <f>_xlfn.CONCAT(O4,O3,O2)</f>
+        <v>1001111111011001011100</v>
+      </c>
+      <c r="N9">
+        <f>P4+P3*2^8+P2*2^16</f>
+        <v>6089807</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -760,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -777,8 +906,18 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11">
+        <f>(N8*10^6)/2^16*(N9)</f>
+        <v>2416000091.5527344</v>
+      </c>
+      <c r="N11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -795,14 +934,24 @@
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>31</v>
+      </c>
+      <c r="M12">
+        <f>M11/10^9</f>
+        <v>2.4160000915527342</v>
+      </c>
+      <c r="N12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="D13">
         <f>LEN(DEC2BIN(LARGE(E2:E12,1)))</f>
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>29</v>
       </c>
@@ -810,7 +959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -821,7 +970,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -963,10 +1112,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D13">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>8</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O6">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>8</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>